<commit_message>
worked on input_new_data function
</commit_message>
<xml_diff>
--- a/prep_and_checklists/DaaniSarma  /PREPLIST_DaaniSarma  _08-05-2025_0.xlsx
+++ b/prep_and_checklists/DaaniSarma  /PREPLIST_DaaniSarma  _08-05-2025_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/DaaniSarma  /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED88089F-2345-DE4E-B156-8ED908BEAD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FB2CBF-6317-644D-9E9D-F705DCE1A6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
   <si>
     <t xml:space="preserve">DaaniSarma  , Guests: 50   , 7:30 PM - 10:30 PM   ,Friday, August 15, 2025  </t>
   </si>
@@ -54,9 +54,6 @@
     <t>brunoise shallots</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>pull / make Seasonal mignonette</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>make / pull lemon vinaigrette</t>
   </si>
   <si>
-    <t>maldon</t>
-  </si>
-  <si>
     <t>olive oil jam</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Beef Tenderloin Canape</t>
   </si>
   <si>
-    <t>Make / portion /pan de mie pullman toast</t>
-  </si>
-  <si>
     <t>clean / portion strip steak</t>
   </si>
   <si>
@@ -213,9 +204,6 @@
     <t>Chives</t>
   </si>
   <si>
-    <t>Chevre</t>
-  </si>
-  <si>
     <t>Yuzu juice</t>
   </si>
   <si>
@@ -352,6 +340,99 @@
   </si>
   <si>
     <t>8:15-10:15 PASSED CANAPÉS</t>
+  </si>
+  <si>
+    <t>1 cup</t>
+  </si>
+  <si>
+    <t>1 pint</t>
+  </si>
+  <si>
+    <t>200pcs</t>
+  </si>
+  <si>
+    <t>4lbs</t>
+  </si>
+  <si>
+    <t>2x recipe</t>
+  </si>
+  <si>
+    <t>1 x squeeze bottle</t>
+  </si>
+  <si>
+    <t>1x recipe</t>
+  </si>
+  <si>
+    <t>1x clam shell</t>
+  </si>
+  <si>
+    <t>1 quart</t>
+  </si>
+  <si>
+    <t>100 pcs</t>
+  </si>
+  <si>
+    <t>120pcs</t>
+  </si>
+  <si>
+    <t>60 pcs, cut in half</t>
+  </si>
+  <si>
+    <t>120 pcs</t>
+  </si>
+  <si>
+    <t>1x loaf</t>
+  </si>
+  <si>
+    <t>Make / portion /brioche pullman toast</t>
+  </si>
+  <si>
+    <t>3 x steaks</t>
+  </si>
+  <si>
+    <t>1/2 x recipe</t>
+  </si>
+  <si>
+    <t>1 x recipe</t>
+  </si>
+  <si>
+    <t>1 pint, * Pull from reach-In freezer</t>
+  </si>
+  <si>
+    <t>2 cups, * Pull from reach-in freezer</t>
+  </si>
+  <si>
+    <t>2x bags</t>
+  </si>
+  <si>
+    <t>1x recipe, in a piping bag</t>
+  </si>
+  <si>
+    <t>8lbs, 2lb increments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 256g </t>
+  </si>
+  <si>
+    <t>3lbs</t>
+  </si>
+  <si>
+    <t>1x3 heads</t>
+  </si>
+  <si>
+    <t>2x "5x5" brioche pullman</t>
+  </si>
+  <si>
+    <t>1 case</t>
+  </si>
+  <si>
+    <t>Basil</t>
+  </si>
+  <si>
+    <t>2.2lbs</t>
+  </si>
+  <si>
+    <t>1x recipe (for both parties)</t>
   </si>
 </sst>
 </file>
@@ -799,10 +880,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B55"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -829,7 +913,7 @@
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B4" s="8"/>
     </row>
@@ -846,36 +930,36 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -883,31 +967,31 @@
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -915,274 +999,266 @@
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
+      <c r="B25" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
+      <c r="B31" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>4</v>
+      <c r="B45" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="B48" s="2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>4</v>
+      <c r="B52" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1267,7 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="77" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1199,13 +1275,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
@@ -1215,412 +1298,429 @@
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="C4" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="C7" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="C13" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="C21" s="5" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="C25" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="C34" s="5" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B45" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="C45" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="C46" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>